<commit_message>
ajustando os espaços do layout
</commit_message>
<xml_diff>
--- a/testelaryssa.xlsx
+++ b/testelaryssa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larissa.barcelos\Desktop\Laryssa\Demandas\conversao excel-txt python para erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66891627-7A24-4670-865B-1E74B31E53D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B08C2C-47F7-4F61-A572-7E1AA4A054C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{646F093E-FCE0-4063-B4F0-739928B612DD}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
-  <si>
-    <t>ACADEMIA DO CORPO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>S</t>
   </si>
@@ -36,18 +33,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>ADM MANTENEDORA</t>
-  </si>
-  <si>
-    <t>ADMINISTRATIVO MANTENEDORA</t>
-  </si>
-  <si>
-    <t>ALMOXARIFADOS</t>
-  </si>
-  <si>
     <t>COD LOCAL</t>
   </si>
   <si>
@@ -70,6 +55,24 @@
   </si>
   <si>
     <t>NOME DO LOCAL</t>
+  </si>
+  <si>
+    <t>301</t>
+  </si>
+  <si>
+    <t>302</t>
+  </si>
+  <si>
+    <t>ACADEMIA TESTE</t>
+  </si>
+  <si>
+    <t>ADM TESTE</t>
+  </si>
+  <si>
+    <t>ALMOXARIFADOS TESTE</t>
+  </si>
+  <si>
+    <t>EMPRESA</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -174,6 +177,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,137 +493,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4B5477-3D35-4F7B-BFED-F163080897F6}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>303</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>2</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="C5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
ajustando o codigo para poder converter na importação das tabelas E670LOC e E670RAT
</commit_message>
<xml_diff>
--- a/testelaryssa.xlsx
+++ b/testelaryssa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larissa.barcelos\Desktop\Laryssa\Demandas\conversao excel-txt python para erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B08C2C-47F7-4F61-A572-7E1AA4A054C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B3E28E-2B48-45B1-A666-94BF0EAC46C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{646F093E-FCE0-4063-B4F0-739928B612DD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>S</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>EMPRESA</t>
+  </si>
+  <si>
+    <t>TROCADO TESTE</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +609,7 @@
         <v>303</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>

</xml_diff>